<commit_message>
Datashetts added and new shopping entered into sheet
</commit_message>
<xml_diff>
--- a/Arduino/Shopping/Sensors.xlsx
+++ b/Arduino/Shopping/Sensors.xlsx
@@ -4,17 +4,18 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13230"/>
+    <workbookView windowWidth="28695" windowHeight="13230" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="August 2016" sheetId="1" r:id="rId1"/>
+    <sheet name="September 2016" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27">
   <si>
     <t>Site</t>
   </si>
@@ -59,6 +60,42 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>0104110000002716</t>
+  </si>
+  <si>
+    <t>Modul WiFi ESP8266 ESP-12E</t>
+  </si>
+  <si>
+    <t>0104110000002150</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Modul DC-DC Step Down LM2596 Albastru Intrare 3 - 40 V </t>
+  </si>
+  <si>
+    <t>0104210000008630</t>
+  </si>
+  <si>
+    <t>L7812 - Stabilizator de Tensiune de 12 V TO-220</t>
+  </si>
+  <si>
+    <t>0104210000008623</t>
+  </si>
+  <si>
+    <t>L7805 - Stabilizator de Tensiune de 5 V TO-220</t>
+  </si>
+  <si>
+    <t>0104110000000576</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Senzor de curent Hall ACS712 (30A) </t>
+  </si>
+  <si>
+    <t>0104110000001481</t>
+  </si>
+  <si>
+    <t>Set de Rezistoare 0.25W 20 de valori câte 20 buc. fiecare</t>
   </si>
 </sst>
 </file>
@@ -66,12 +103,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -88,6 +125,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -96,6 +140,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -105,21 +165,6 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -133,8 +178,91 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -148,53 +276,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -207,30 +291,6 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -241,19 +301,85 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,13 +397,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -289,37 +415,55 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -331,97 +475,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -459,6 +519,17 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -470,30 +541,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -522,13 +569,26 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
+      <top/>
       <bottom style="double">
-        <color theme="4"/>
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -537,7 +597,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -555,149 +615,182 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="7" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="8" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="10">
-      <alignment vertical="center"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="10">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="10">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -706,9 +799,6 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1027,13 +1117,13 @@
   <sheetPr/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E11" sqref="A1:E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="17.125" style="1" customWidth="1"/>
+    <col min="1" max="1" width="17.125" style="13" customWidth="1"/>
     <col min="2" max="2" width="69.5" customWidth="1"/>
     <col min="3" max="3" width="11.125" customWidth="1"/>
     <col min="4" max="4" width="12.25" customWidth="1"/>
@@ -1041,7 +1131,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
@@ -1049,127 +1139,325 @@
       </c>
     </row>
     <row r="2" spans="1:2">
-      <c r="A2" s="1" t="s">
+      <c r="A2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="15" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:5">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B4" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="D4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="4" t="s">
+      <c r="E4" s="7" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:5">
-      <c r="A5" s="5">
+      <c r="A5" s="16">
         <v>104110000003188</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="17">
         <v>1</v>
       </c>
-      <c r="D5" s="7">
+      <c r="D5" s="18">
         <v>11.99</v>
       </c>
-      <c r="E5" s="7">
-        <f>C5*D5</f>
+      <c r="E5" s="18">
+        <f t="shared" ref="E5:E9" si="0">C5*D5</f>
         <v>11.99</v>
       </c>
     </row>
     <row r="6" spans="1:5">
-      <c r="A6" s="5">
+      <c r="A6" s="16">
         <v>104210000005943</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="17">
         <v>2</v>
       </c>
-      <c r="D6" s="7">
+      <c r="D6" s="18">
         <v>5.95</v>
       </c>
-      <c r="E6" s="7">
-        <f>C6*D6</f>
+      <c r="E6" s="18">
+        <f t="shared" si="0"/>
         <v>11.9</v>
       </c>
     </row>
     <row r="7" spans="1:5">
-      <c r="A7" s="5">
+      <c r="A7" s="16">
         <v>104110000008503</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="17">
         <v>1</v>
       </c>
-      <c r="D7" s="7">
+      <c r="D7" s="18">
         <v>24.99</v>
       </c>
-      <c r="E7" s="7">
-        <f>C7*D7</f>
+      <c r="E7" s="18">
+        <f t="shared" si="0"/>
         <v>24.99</v>
       </c>
     </row>
     <row r="8" spans="1:5">
-      <c r="A8" s="5">
+      <c r="A8" s="16">
         <v>104110000016300</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="17">
         <v>2</v>
       </c>
-      <c r="D8" s="7">
+      <c r="D8" s="18">
         <v>15.99</v>
       </c>
-      <c r="E8" s="7">
-        <f>C8*D8</f>
+      <c r="E8" s="18">
+        <f t="shared" si="0"/>
         <v>31.98</v>
       </c>
     </row>
     <row r="9" spans="1:5">
-      <c r="A9" s="5">
+      <c r="A9" s="16">
         <v>104210000002096</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="17">
         <v>2</v>
       </c>
-      <c r="D9" s="7">
+      <c r="D9" s="18">
         <v>0.95</v>
       </c>
-      <c r="E9" s="7">
-        <f>C9*D9</f>
+      <c r="E9" s="18">
+        <f t="shared" si="0"/>
         <v>1.9</v>
       </c>
     </row>
     <row r="11" spans="4:5">
-      <c r="D11" s="8" t="s">
+      <c r="D11" s="11" t="s">
         <v>14</v>
       </c>
       <c r="E11">
         <f>SUM(E5:E9)</f>
         <v>82.76</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://github.com/ThunderWorm/makerspace/tree/master/Arduino/DataSheets"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:E12"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="4"/>
+  <cols>
+    <col min="1" max="1" width="20.625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="69.5" customWidth="1"/>
+    <col min="3" max="3" width="7.75" customWidth="1"/>
+    <col min="4" max="4" width="8.875" customWidth="1"/>
+    <col min="5" max="5" width="7.875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="3"/>
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="7" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="9">
+        <v>17.99</v>
+      </c>
+      <c r="E5" s="9">
+        <f>C5*D5</f>
+        <v>17.99</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="8">
+        <v>1</v>
+      </c>
+      <c r="D6" s="9">
+        <v>7.99</v>
+      </c>
+      <c r="E6" s="9">
+        <f>C6*D6</f>
+        <v>7.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="8">
+        <v>1</v>
+      </c>
+      <c r="D7" s="9">
+        <v>1.99</v>
+      </c>
+      <c r="E7" s="9">
+        <f>C7*D7</f>
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="8">
+        <v>1</v>
+      </c>
+      <c r="D8" s="9">
+        <v>1.99</v>
+      </c>
+      <c r="E8" s="9">
+        <f>C8*D8</f>
+        <v>1.99</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" s="10" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C9" s="8">
+        <v>1</v>
+      </c>
+      <c r="D9" s="9">
+        <v>17.95</v>
+      </c>
+      <c r="E9" s="9">
+        <f>C9*D9</f>
+        <v>17.95</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="3">
+        <v>1</v>
+      </c>
+      <c r="D10" s="3">
+        <f>7.48</f>
+        <v>7.48</v>
+      </c>
+      <c r="E10" s="9">
+        <f>C10*D10</f>
+        <v>7.48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="11"/>
+      <c r="E11" s="3"/>
+    </row>
+    <row r="12" spans="4:5">
+      <c r="D12" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="E12">
+        <f>SUM(E5:E10)</f>
+        <v>55.39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>